<commit_message>
Cluster | kyc file -v4
</commit_message>
<xml_diff>
--- a/Data/inputs.xlsx
+++ b/Data/inputs.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="26775" windowHeight="13290"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="26775" windowHeight="13290" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="TRAN" sheetId="2" r:id="rId1"/>
+    <sheet name="KYC" sheetId="3" r:id="rId2"/>
+    <sheet name="TRAN_CLUSTER" sheetId="4" r:id="rId3"/>
+    <sheet name="KYC_CLUSTER" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="94">
   <si>
     <t>TRAN_DT</t>
   </si>
@@ -129,13 +131,182 @@
   </si>
   <si>
     <t>Kingsley</t>
+  </si>
+  <si>
+    <t>AVE_BAL</t>
+  </si>
+  <si>
+    <t>AVE_TXN</t>
+  </si>
+  <si>
+    <t>CLUSTER</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>MARITAL</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>OCCUPATION</t>
+  </si>
+  <si>
+    <t>C11122200</t>
+  </si>
+  <si>
+    <t>C11122201</t>
+  </si>
+  <si>
+    <t>C11122202</t>
+  </si>
+  <si>
+    <t>C11122203</t>
+  </si>
+  <si>
+    <t>C11122204</t>
+  </si>
+  <si>
+    <t>C11122205</t>
+  </si>
+  <si>
+    <t>C11122206</t>
+  </si>
+  <si>
+    <t>C11122207</t>
+  </si>
+  <si>
+    <t>C11122208</t>
+  </si>
+  <si>
+    <t>C11122209</t>
+  </si>
+  <si>
+    <t>C11122210</t>
+  </si>
+  <si>
+    <t>C11122211</t>
+  </si>
+  <si>
+    <t>P.O. Box 281, 7465 Enim. Road</t>
+  </si>
+  <si>
+    <t>P.O. Box 685, 3082 Dolor Rd.</t>
+  </si>
+  <si>
+    <t>5151 Pede. Ave</t>
+  </si>
+  <si>
+    <t>P.O. Box 284, 5405 Quam. Road</t>
+  </si>
+  <si>
+    <t>Ap #273-3220 Condimentum Rd.</t>
+  </si>
+  <si>
+    <t>932-1988 Augue Street</t>
+  </si>
+  <si>
+    <t>P.O. Box 663, 505 In St.</t>
+  </si>
+  <si>
+    <t>326-4585 Mauris Av.</t>
+  </si>
+  <si>
+    <t>Ap #976-1176 Malesuada Avenue</t>
+  </si>
+  <si>
+    <t>650-6823 Fringilla Rd.</t>
+  </si>
+  <si>
+    <t>1220 Walker Rd.</t>
+  </si>
+  <si>
+    <t>88 Wall Street</t>
+  </si>
+  <si>
+    <t>Knoxville</t>
+  </si>
+  <si>
+    <t>Cincinnati</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Springdale</t>
+  </si>
+  <si>
+    <t>Bear</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Newark</t>
+  </si>
+  <si>
+    <t>Warren</t>
+  </si>
+  <si>
+    <t>Kansas City</t>
+  </si>
+  <si>
+    <t>Olympia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>&lt;30k</t>
+  </si>
+  <si>
+    <t>500k to 1M</t>
+  </si>
+  <si>
+    <t>&gt;1.25M</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>STUDENT</t>
+  </si>
+  <si>
+    <t>INTERN</t>
+  </si>
+  <si>
+    <t>SINGLE</t>
+  </si>
+  <si>
+    <t>MARRIED</t>
+  </si>
+  <si>
+    <t>PROFESSOR</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>DIRECTOR</t>
+  </si>
+  <si>
+    <t>DENTIST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -155,41 +326,20 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor theme="4" tint="0.59999389629810485"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -204,13 +354,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
     <dxf>
       <font>
         <b val="0"/>
@@ -227,6 +377,31 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     </dxf>
     <dxf>
       <font>
@@ -244,7 +419,28 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="33" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -303,22 +499,96 @@
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="33" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G372" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowCellStyle="Comma" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G372" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Comma" dataCellStyle="Comma">
   <autoFilter ref="A1:G372"/>
   <tableColumns count="7">
     <tableColumn id="1" name="TRAN_ID"/>
-    <tableColumn id="2" name="TRAN_DT" dataDxfId="5"/>
+    <tableColumn id="2" name="TRAN_DT" dataDxfId="6"/>
     <tableColumn id="3" name="ACC_ID"/>
     <tableColumn id="4" name="TRAN_REMARKS"/>
-    <tableColumn id="5" name="WITHDRAWAL" dataDxfId="4" dataCellStyle="Comma"/>
-    <tableColumn id="6" name="DEPOSIT" dataDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="BALANCE" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="5" name="WITHDRAWAL" dataDxfId="5" dataCellStyle="Comma"/>
+    <tableColumn id="6" name="DEPOSIT" dataDxfId="4" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="BALANCE" dataDxfId="3" dataCellStyle="Comma"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:L13" totalsRowShown="0">
+  <autoFilter ref="A1:L13">
+    <filterColumn colId="8"/>
+    <filterColumn colId="9"/>
+    <filterColumn colId="10"/>
+    <filterColumn colId="11"/>
+  </autoFilter>
+  <tableColumns count="12">
+    <tableColumn id="1" name="ACC_ID" dataDxfId="0"/>
+    <tableColumn id="2" name="SSN"/>
+    <tableColumn id="3" name="FIRST_NAME"/>
+    <tableColumn id="4" name="LAST_NAME"/>
+    <tableColumn id="5" name="PASSPORT"/>
+    <tableColumn id="6" name="ADDRESS"/>
+    <tableColumn id="7" name="CITY"/>
+    <tableColumn id="8" name="COUNTRY"/>
+    <tableColumn id="9" name="AGE"/>
+    <tableColumn id="10" name="MARITAL"/>
+    <tableColumn id="11" name="GENDER"/>
+    <tableColumn id="12" name="OCCUPATION"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D13" totalsRowShown="0">
+  <autoFilter ref="A1:D13"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="ACC_ID" dataDxfId="2"/>
+    <tableColumn id="2" name="CLUSTER"/>
+    <tableColumn id="3" name="AVE_BAL"/>
+    <tableColumn id="4" name="AVE_TXN" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -611,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="F369" sqref="F369"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C256" sqref="C256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3446,7 +3716,7 @@
         <v>25000</v>
       </c>
       <c r="G141" s="2">
-        <v>225000</v>
+        <v>725000</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -3466,7 +3736,7 @@
         <v>8500</v>
       </c>
       <c r="G142" s="2">
-        <v>233500</v>
+        <v>733500</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -3486,7 +3756,7 @@
         <v>575</v>
       </c>
       <c r="G143" s="2">
-        <v>232925</v>
+        <v>732925</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -3506,7 +3776,7 @@
         <v>1000</v>
       </c>
       <c r="G144" s="2">
-        <v>231925</v>
+        <v>731925</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -3526,7 +3796,7 @@
         <v>18000</v>
       </c>
       <c r="G145" s="2">
-        <v>249925</v>
+        <v>749925</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -3546,7 +3816,7 @@
         <v>425</v>
       </c>
       <c r="G146" s="2">
-        <v>249500</v>
+        <v>749500</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -3566,7 +3836,7 @@
         <v>627</v>
       </c>
       <c r="G147" s="2">
-        <v>248873</v>
+        <v>748873</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -3586,7 +3856,7 @@
         <v>25</v>
       </c>
       <c r="G148" s="2">
-        <v>248898</v>
+        <v>748898</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -3606,7 +3876,7 @@
         <v>1000</v>
       </c>
       <c r="G149" s="2">
-        <v>247898</v>
+        <v>747898</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -3626,7 +3896,7 @@
         <v>12000</v>
       </c>
       <c r="G150" s="2">
-        <v>259898</v>
+        <v>759898</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -3646,7 +3916,7 @@
         <v>1000</v>
       </c>
       <c r="G151" s="2">
-        <v>258898</v>
+        <v>758898</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -3666,7 +3936,7 @@
         <v>64000</v>
       </c>
       <c r="G152" s="2">
-        <v>194898</v>
+        <v>694898</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -3686,7 +3956,7 @@
         <v>29000</v>
       </c>
       <c r="G153" s="2">
-        <v>165898</v>
+        <v>665898</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -3706,7 +3976,7 @@
         <v>250</v>
       </c>
       <c r="G154" s="2">
-        <v>166148</v>
+        <v>666148</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -3726,7 +3996,7 @@
         <v>1000</v>
       </c>
       <c r="G155" s="2">
-        <v>165148</v>
+        <v>665148</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -3746,7 +4016,7 @@
         <v>212</v>
       </c>
       <c r="G156" s="2">
-        <v>164936</v>
+        <v>664936</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -3766,7 +4036,7 @@
         <v>22000</v>
       </c>
       <c r="G157" s="2">
-        <v>186936</v>
+        <v>686936</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -3786,7 +4056,7 @@
         <v>120000</v>
       </c>
       <c r="G158" s="2">
-        <v>66936</v>
+        <v>566936</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -3806,7 +4076,7 @@
         <v>75000</v>
       </c>
       <c r="G159" s="2">
-        <v>141936</v>
+        <v>641936</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -3826,7 +4096,7 @@
         <v>1000</v>
       </c>
       <c r="G160" s="2">
-        <v>140936</v>
+        <v>640936</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -3846,7 +4116,7 @@
         <v>80</v>
       </c>
       <c r="G161" s="2">
-        <v>140856</v>
+        <v>640856</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -3866,7 +4136,7 @@
         <v>16000</v>
       </c>
       <c r="G162" s="2">
-        <v>124856</v>
+        <v>624856</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -3886,7 +4156,7 @@
         <v>650</v>
       </c>
       <c r="G163" s="2">
-        <v>125506</v>
+        <v>625506</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -3906,7 +4176,7 @@
         <v>1000</v>
       </c>
       <c r="G164" s="2">
-        <v>124506</v>
+        <v>624506</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -3926,7 +4196,7 @@
         <v>56</v>
       </c>
       <c r="G165" s="2">
-        <v>124450</v>
+        <v>624450</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -3946,7 +4216,7 @@
         <v>6000</v>
       </c>
       <c r="G166" s="2">
-        <v>118450</v>
+        <v>618450</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -3966,7 +4236,7 @@
         <v>22000</v>
       </c>
       <c r="G167" s="2">
-        <v>140450</v>
+        <v>640450</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -3986,7 +4256,7 @@
         <v>850</v>
       </c>
       <c r="G168" s="2">
-        <v>141300</v>
+        <v>641300</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -4006,7 +4276,7 @@
         <v>48000</v>
       </c>
       <c r="G169" s="2">
-        <v>93300</v>
+        <v>593300</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -4026,7 +4296,7 @@
         <v>25000</v>
       </c>
       <c r="G170" s="2">
-        <v>295000</v>
+        <v>795000</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -4046,7 +4316,7 @@
         <v>8500</v>
       </c>
       <c r="G171" s="2">
-        <v>303500</v>
+        <v>803500</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -4066,7 +4336,7 @@
         <v>5750</v>
       </c>
       <c r="G172" s="2">
-        <v>297750</v>
+        <v>797750</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -4086,7 +4356,7 @@
         <v>1000</v>
       </c>
       <c r="G173" s="2">
-        <v>296750</v>
+        <v>796750</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -4106,7 +4376,7 @@
         <v>18000</v>
       </c>
       <c r="G174" s="2">
-        <v>314750</v>
+        <v>814750</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -4126,7 +4396,7 @@
         <v>40000</v>
       </c>
       <c r="G175" s="2">
-        <v>274750</v>
+        <v>774750</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -4146,7 +4416,7 @@
         <v>6270</v>
       </c>
       <c r="G176" s="2">
-        <v>268480</v>
+        <v>768480</v>
       </c>
     </row>
     <row r="177" spans="1:7">
@@ -4166,7 +4436,7 @@
         <v>82000</v>
       </c>
       <c r="G177" s="2">
-        <v>350480</v>
+        <v>850480</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -4186,7 +4456,7 @@
         <v>1000</v>
       </c>
       <c r="G178" s="2">
-        <v>349480</v>
+        <v>849480</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -4206,7 +4476,7 @@
         <v>12000</v>
       </c>
       <c r="G179" s="2">
-        <v>361480</v>
+        <v>861480</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -4226,7 +4496,7 @@
         <v>1000</v>
       </c>
       <c r="G180" s="2">
-        <v>360480</v>
+        <v>860480</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -4246,7 +4516,7 @@
         <v>64000</v>
       </c>
       <c r="G181" s="2">
-        <v>296480</v>
+        <v>796480</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -4266,7 +4536,7 @@
         <v>29000</v>
       </c>
       <c r="G182" s="2">
-        <v>267480</v>
+        <v>767480</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -4286,7 +4556,7 @@
         <v>1500</v>
       </c>
       <c r="G183" s="2">
-        <v>268980</v>
+        <v>768980</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -4306,7 +4576,7 @@
         <v>18000</v>
       </c>
       <c r="G184" s="2">
-        <v>250980</v>
+        <v>750980</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -4326,7 +4596,7 @@
         <v>212</v>
       </c>
       <c r="G185" s="2">
-        <v>250768</v>
+        <v>750768</v>
       </c>
     </row>
     <row r="186" spans="1:7">
@@ -4346,7 +4616,7 @@
         <v>22000</v>
       </c>
       <c r="G186" s="2">
-        <v>272768</v>
+        <v>772768</v>
       </c>
     </row>
     <row r="187" spans="1:7">
@@ -4366,7 +4636,7 @@
         <v>120000</v>
       </c>
       <c r="G187" s="2">
-        <v>152768</v>
+        <v>652768</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -4386,7 +4656,7 @@
         <v>75000</v>
       </c>
       <c r="G188" s="2">
-        <v>227768</v>
+        <v>727768</v>
       </c>
     </row>
     <row r="189" spans="1:7">
@@ -4406,7 +4676,7 @@
         <v>1000</v>
       </c>
       <c r="G189" s="2">
-        <v>226768</v>
+        <v>726768</v>
       </c>
     </row>
     <row r="190" spans="1:7">
@@ -4426,7 +4696,7 @@
         <v>80200</v>
       </c>
       <c r="G190" s="2">
-        <v>146568</v>
+        <v>646568</v>
       </c>
     </row>
     <row r="191" spans="1:7">
@@ -4446,7 +4716,7 @@
         <v>16000</v>
       </c>
       <c r="G191" s="2">
-        <v>130568</v>
+        <v>630568</v>
       </c>
     </row>
     <row r="192" spans="1:7">
@@ -4466,7 +4736,7 @@
         <v>650</v>
       </c>
       <c r="G192" s="2">
-        <v>131218</v>
+        <v>631218</v>
       </c>
     </row>
     <row r="193" spans="1:7">
@@ -4486,7 +4756,7 @@
         <v>10000</v>
       </c>
       <c r="G193" s="2">
-        <v>121218</v>
+        <v>621218</v>
       </c>
     </row>
     <row r="194" spans="1:7">
@@ -4506,7 +4776,7 @@
         <v>8500</v>
       </c>
       <c r="G194" s="2">
-        <v>112718</v>
+        <v>612718</v>
       </c>
     </row>
     <row r="195" spans="1:7">
@@ -4526,7 +4796,7 @@
         <v>6000</v>
       </c>
       <c r="G195" s="2">
-        <v>106718</v>
+        <v>606718</v>
       </c>
     </row>
     <row r="196" spans="1:7">
@@ -4546,7 +4816,7 @@
         <v>22000</v>
       </c>
       <c r="G196" s="2">
-        <v>128718</v>
+        <v>628718</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -4566,7 +4836,7 @@
         <v>12000</v>
       </c>
       <c r="G197" s="2">
-        <v>140718</v>
+        <v>640718</v>
       </c>
     </row>
     <row r="198" spans="1:7">
@@ -4586,7 +4856,7 @@
         <v>48000</v>
       </c>
       <c r="G198" s="2">
-        <v>92718</v>
+        <v>592718</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -4606,7 +4876,7 @@
         <v>25000</v>
       </c>
       <c r="G199" s="2">
-        <v>455000</v>
+        <v>955000</v>
       </c>
     </row>
     <row r="200" spans="1:7">
@@ -4626,7 +4896,7 @@
         <v>8500</v>
       </c>
       <c r="G200" s="2">
-        <v>463500</v>
+        <v>963500</v>
       </c>
     </row>
     <row r="201" spans="1:7">
@@ -4646,7 +4916,7 @@
         <v>44000</v>
       </c>
       <c r="G201" s="2">
-        <v>419500</v>
+        <v>919500</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -4666,7 +4936,7 @@
         <v>1000</v>
       </c>
       <c r="G202" s="2">
-        <v>418500</v>
+        <v>918500</v>
       </c>
     </row>
     <row r="203" spans="1:7">
@@ -4686,7 +4956,7 @@
         <v>18000</v>
       </c>
       <c r="G203" s="2">
-        <v>436500</v>
+        <v>936500</v>
       </c>
     </row>
     <row r="204" spans="1:7">
@@ -4706,7 +4976,7 @@
         <v>40000</v>
       </c>
       <c r="G204" s="2">
-        <v>396500</v>
+        <v>896500</v>
       </c>
     </row>
     <row r="205" spans="1:7">
@@ -4726,7 +4996,7 @@
         <v>62000</v>
       </c>
       <c r="G205" s="2">
-        <v>334500</v>
+        <v>834500</v>
       </c>
     </row>
     <row r="206" spans="1:7">
@@ -4746,7 +5016,7 @@
         <v>82000</v>
       </c>
       <c r="G206" s="2">
-        <v>416500</v>
+        <v>916500</v>
       </c>
     </row>
     <row r="207" spans="1:7">
@@ -4766,7 +5036,7 @@
         <v>1000</v>
       </c>
       <c r="G207" s="2">
-        <v>415500</v>
+        <v>915500</v>
       </c>
     </row>
     <row r="208" spans="1:7">
@@ -4786,7 +5056,7 @@
         <v>12000</v>
       </c>
       <c r="G208" s="2">
-        <v>427500</v>
+        <v>927500</v>
       </c>
     </row>
     <row r="209" spans="1:7">
@@ -4806,7 +5076,7 @@
         <v>1000</v>
       </c>
       <c r="G209" s="2">
-        <v>426500</v>
+        <v>926500</v>
       </c>
     </row>
     <row r="210" spans="1:7">
@@ -4826,7 +5096,7 @@
         <v>64000</v>
       </c>
       <c r="G210" s="2">
-        <v>362500</v>
+        <v>862500</v>
       </c>
     </row>
     <row r="211" spans="1:7">
@@ -4846,7 +5116,7 @@
         <v>29000</v>
       </c>
       <c r="G211" s="2">
-        <v>333500</v>
+        <v>833500</v>
       </c>
     </row>
     <row r="212" spans="1:7">
@@ -4866,7 +5136,7 @@
         <v>125000</v>
       </c>
       <c r="G212" s="2">
-        <v>458500</v>
+        <v>958500</v>
       </c>
     </row>
     <row r="213" spans="1:7">
@@ -4886,7 +5156,7 @@
         <v>180000</v>
       </c>
       <c r="G213" s="2">
-        <v>278500</v>
+        <v>778500</v>
       </c>
     </row>
     <row r="214" spans="1:7">
@@ -4906,7 +5176,7 @@
         <v>212</v>
       </c>
       <c r="G214" s="2">
-        <v>278288</v>
+        <v>778288</v>
       </c>
     </row>
     <row r="215" spans="1:7">
@@ -4926,7 +5196,7 @@
         <v>22000</v>
       </c>
       <c r="G215" s="2">
-        <v>300288</v>
+        <v>800288</v>
       </c>
     </row>
     <row r="216" spans="1:7">
@@ -4946,7 +5216,7 @@
         <v>120000</v>
       </c>
       <c r="G216" s="2">
-        <v>180288</v>
+        <v>680288</v>
       </c>
     </row>
     <row r="217" spans="1:7">
@@ -4966,7 +5236,7 @@
         <v>75000</v>
       </c>
       <c r="G217" s="2">
-        <v>255288</v>
+        <v>755288</v>
       </c>
     </row>
     <row r="218" spans="1:7">
@@ -4986,7 +5256,7 @@
         <v>1000</v>
       </c>
       <c r="G218" s="2">
-        <v>254288</v>
+        <v>754288</v>
       </c>
     </row>
     <row r="219" spans="1:7">
@@ -5006,7 +5276,7 @@
         <v>80200</v>
       </c>
       <c r="G219" s="2">
-        <v>174088</v>
+        <v>674088</v>
       </c>
     </row>
     <row r="220" spans="1:7">
@@ -5026,7 +5296,7 @@
         <v>16000</v>
       </c>
       <c r="G220" s="2">
-        <v>158088</v>
+        <v>658088</v>
       </c>
     </row>
     <row r="221" spans="1:7">
@@ -5046,7 +5316,7 @@
         <v>50000</v>
       </c>
       <c r="G221" s="2">
-        <v>208088</v>
+        <v>708088</v>
       </c>
     </row>
     <row r="222" spans="1:7">
@@ -5066,7 +5336,7 @@
         <v>10000</v>
       </c>
       <c r="G222" s="2">
-        <v>198088</v>
+        <v>698088</v>
       </c>
     </row>
     <row r="223" spans="1:7">
@@ -5086,7 +5356,7 @@
         <v>85000</v>
       </c>
       <c r="G223" s="2">
-        <v>113088</v>
+        <v>613088</v>
       </c>
     </row>
     <row r="224" spans="1:7">
@@ -5106,7 +5376,7 @@
         <v>6000</v>
       </c>
       <c r="G224" s="2">
-        <v>107088</v>
+        <v>607088</v>
       </c>
     </row>
     <row r="225" spans="1:7">
@@ -5126,7 +5396,7 @@
         <v>220000</v>
       </c>
       <c r="G225" s="2">
-        <v>327088</v>
+        <v>827088</v>
       </c>
     </row>
     <row r="226" spans="1:7">
@@ -5146,7 +5416,7 @@
         <v>12000</v>
       </c>
       <c r="G226" s="2">
-        <v>339088</v>
+        <v>839088</v>
       </c>
     </row>
     <row r="227" spans="1:7">
@@ -5166,7 +5436,7 @@
         <v>48000</v>
       </c>
       <c r="G227" s="2">
-        <v>291088</v>
+        <v>791088</v>
       </c>
     </row>
     <row r="228" spans="1:7">
@@ -5186,7 +5456,7 @@
         <v>25000</v>
       </c>
       <c r="G228" s="2">
-        <v>325000</v>
+        <v>825000</v>
       </c>
     </row>
     <row r="229" spans="1:7">
@@ -5206,7 +5476,7 @@
         <v>8500</v>
       </c>
       <c r="G229" s="2">
-        <v>333500</v>
+        <v>833500</v>
       </c>
     </row>
     <row r="230" spans="1:7">
@@ -5226,7 +5496,7 @@
         <v>44000</v>
       </c>
       <c r="G230" s="2">
-        <v>289500</v>
+        <v>789500</v>
       </c>
     </row>
     <row r="231" spans="1:7">
@@ -5246,7 +5516,7 @@
         <v>1000</v>
       </c>
       <c r="G231" s="2">
-        <v>288500</v>
+        <v>788500</v>
       </c>
     </row>
     <row r="232" spans="1:7">
@@ -5266,7 +5536,7 @@
         <v>16500</v>
       </c>
       <c r="G232" s="2">
-        <v>305000</v>
+        <v>805000</v>
       </c>
     </row>
     <row r="233" spans="1:7">
@@ -5286,7 +5556,7 @@
         <v>40000</v>
       </c>
       <c r="G233" s="2">
-        <v>265000</v>
+        <v>765000</v>
       </c>
     </row>
     <row r="234" spans="1:7">
@@ -5306,7 +5576,7 @@
         <v>62000</v>
       </c>
       <c r="G234" s="2">
-        <v>203000</v>
+        <v>703000</v>
       </c>
     </row>
     <row r="235" spans="1:7">
@@ -5326,7 +5596,7 @@
         <v>81500</v>
       </c>
       <c r="G235" s="2">
-        <v>284500</v>
+        <v>784500</v>
       </c>
     </row>
     <row r="236" spans="1:7">
@@ -5346,7 +5616,7 @@
         <v>720</v>
       </c>
       <c r="G236" s="2">
-        <v>283780</v>
+        <v>783780</v>
       </c>
     </row>
     <row r="237" spans="1:7">
@@ -5366,7 +5636,7 @@
         <v>13600</v>
       </c>
       <c r="G237" s="2">
-        <v>297380</v>
+        <v>797380</v>
       </c>
     </row>
     <row r="238" spans="1:7">
@@ -5386,7 +5656,7 @@
         <v>1800</v>
       </c>
       <c r="G238" s="2">
-        <v>295580</v>
+        <v>795580</v>
       </c>
     </row>
     <row r="239" spans="1:7">
@@ -5406,7 +5676,7 @@
         <v>64000</v>
       </c>
       <c r="G239" s="2">
-        <v>231580</v>
+        <v>731580</v>
       </c>
     </row>
     <row r="240" spans="1:7">
@@ -5426,7 +5696,7 @@
         <v>29000</v>
       </c>
       <c r="G240" s="2">
-        <v>202580</v>
+        <v>702580</v>
       </c>
     </row>
     <row r="241" spans="1:7">
@@ -5446,7 +5716,7 @@
         <v>125000</v>
       </c>
       <c r="G241" s="2">
-        <v>327580</v>
+        <v>827580</v>
       </c>
     </row>
     <row r="242" spans="1:7">
@@ -5466,7 +5736,7 @@
         <v>180000</v>
       </c>
       <c r="G242" s="2">
-        <v>147580</v>
+        <v>647580</v>
       </c>
     </row>
     <row r="243" spans="1:7">
@@ -5486,7 +5756,7 @@
         <v>212</v>
       </c>
       <c r="G243" s="2">
-        <v>147368</v>
+        <v>647368</v>
       </c>
     </row>
     <row r="244" spans="1:7">
@@ -5506,7 +5776,7 @@
         <v>22000</v>
       </c>
       <c r="G244" s="2">
-        <v>169368</v>
+        <v>669368</v>
       </c>
     </row>
     <row r="245" spans="1:7">
@@ -5526,7 +5796,7 @@
         <v>120000</v>
       </c>
       <c r="G245" s="2">
-        <v>49368</v>
+        <v>549368</v>
       </c>
     </row>
     <row r="246" spans="1:7">
@@ -5546,7 +5816,7 @@
         <v>75000</v>
       </c>
       <c r="G246" s="2">
-        <v>124368</v>
+        <v>624368</v>
       </c>
     </row>
     <row r="247" spans="1:7">
@@ -5566,7 +5836,7 @@
         <v>8500</v>
       </c>
       <c r="G247" s="2">
-        <v>115868</v>
+        <v>615868</v>
       </c>
     </row>
     <row r="248" spans="1:7">
@@ -5586,7 +5856,7 @@
         <v>18500</v>
       </c>
       <c r="G248" s="2">
-        <v>97368</v>
+        <v>597368</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -5606,7 +5876,7 @@
         <v>14400</v>
       </c>
       <c r="G249" s="2">
-        <v>82968</v>
+        <v>582968</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -5626,7 +5896,7 @@
         <v>120000</v>
       </c>
       <c r="G250" s="2">
-        <v>202968</v>
+        <v>702968</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -5646,7 +5916,7 @@
         <v>10000</v>
       </c>
       <c r="G251" s="2">
-        <v>192968</v>
+        <v>692968</v>
       </c>
     </row>
     <row r="252" spans="1:7">
@@ -5666,7 +5936,7 @@
         <v>85000</v>
       </c>
       <c r="G252" s="2">
-        <v>107968</v>
+        <v>607968</v>
       </c>
     </row>
     <row r="253" spans="1:7">
@@ -5686,7 +5956,7 @@
         <v>6000</v>
       </c>
       <c r="G253" s="2">
-        <v>101968</v>
+        <v>601968</v>
       </c>
     </row>
     <row r="254" spans="1:7">
@@ -5706,7 +5976,7 @@
         <v>2200</v>
       </c>
       <c r="G254" s="2">
-        <v>104168</v>
+        <v>604168</v>
       </c>
     </row>
     <row r="255" spans="1:7">
@@ -5726,7 +5996,7 @@
         <v>12000</v>
       </c>
       <c r="G255" s="2">
-        <v>116168</v>
+        <v>616168</v>
       </c>
     </row>
     <row r="256" spans="1:7">
@@ -5746,7 +6016,7 @@
         <v>48000</v>
       </c>
       <c r="G256" s="2">
-        <v>68168</v>
+        <v>568168</v>
       </c>
     </row>
     <row r="257" spans="1:7">
@@ -5766,7 +6036,7 @@
         <v>1000000</v>
       </c>
       <c r="G257" s="2">
-        <v>7000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="258" spans="1:7">
@@ -5786,7 +6056,7 @@
         <v>850000</v>
       </c>
       <c r="G258" s="2">
-        <v>7850000</v>
+        <v>1850000</v>
       </c>
     </row>
     <row r="259" spans="1:7">
@@ -5806,7 +6076,7 @@
         <v>44000</v>
       </c>
       <c r="G259" s="2">
-        <v>7806000</v>
+        <v>1806000</v>
       </c>
     </row>
     <row r="260" spans="1:7">
@@ -5826,7 +6096,7 @@
         <v>100000</v>
       </c>
       <c r="G260" s="2">
-        <v>7706000</v>
+        <v>1706000</v>
       </c>
     </row>
     <row r="261" spans="1:7">
@@ -5846,7 +6116,7 @@
         <v>165000</v>
       </c>
       <c r="G261" s="2">
-        <v>7871000</v>
+        <v>1871000</v>
       </c>
     </row>
     <row r="262" spans="1:7">
@@ -5866,7 +6136,7 @@
         <v>40000</v>
       </c>
       <c r="G262" s="2">
-        <v>7831000</v>
+        <v>1831000</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -5886,7 +6156,7 @@
         <v>62000</v>
       </c>
       <c r="G263" s="2">
-        <v>7769000</v>
+        <v>1769000</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -5906,7 +6176,7 @@
         <v>815000</v>
       </c>
       <c r="G264" s="2">
-        <v>8584000</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -5926,7 +6196,7 @@
         <v>250000</v>
       </c>
       <c r="G265" s="2">
-        <v>8334000</v>
+        <v>2334000</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -5943,10 +6213,10 @@
         <v>7</v>
       </c>
       <c r="F266" s="2">
-        <v>3000000</v>
+        <v>250000</v>
       </c>
       <c r="G266" s="2">
-        <v>11334000</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -5966,7 +6236,7 @@
         <v>180025</v>
       </c>
       <c r="G267" s="2">
-        <v>11153975</v>
+        <v>2403975</v>
       </c>
     </row>
     <row r="268" spans="1:7">
@@ -5986,7 +6256,7 @@
         <v>64000</v>
       </c>
       <c r="G268" s="2">
-        <v>11089975</v>
+        <v>2339975</v>
       </c>
     </row>
     <row r="269" spans="1:7">
@@ -6006,7 +6276,7 @@
         <v>29000</v>
       </c>
       <c r="G269" s="2">
-        <v>11060975</v>
+        <v>2310975</v>
       </c>
     </row>
     <row r="270" spans="1:7">
@@ -6026,7 +6296,7 @@
         <v>125000</v>
       </c>
       <c r="G270" s="2">
-        <v>11185975</v>
+        <v>2435975</v>
       </c>
     </row>
     <row r="271" spans="1:7">
@@ -6046,7 +6316,7 @@
         <v>1800000</v>
       </c>
       <c r="G271" s="2">
-        <v>9385975</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="272" spans="1:7">
@@ -6066,7 +6336,7 @@
         <v>25000</v>
       </c>
       <c r="G272" s="2">
-        <v>9360975</v>
+        <v>2334000</v>
       </c>
     </row>
     <row r="273" spans="1:7">
@@ -6086,7 +6356,7 @@
         <v>2200000</v>
       </c>
       <c r="G273" s="2">
-        <v>11560975</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="274" spans="1:7">
@@ -6106,7 +6376,7 @@
         <v>120000</v>
       </c>
       <c r="G274" s="2">
-        <v>11440975</v>
+        <v>2690975</v>
       </c>
     </row>
     <row r="275" spans="1:7">
@@ -6126,7 +6396,7 @@
         <v>75000</v>
       </c>
       <c r="G275" s="2">
-        <v>11515975</v>
+        <v>2765975</v>
       </c>
     </row>
     <row r="276" spans="1:7">
@@ -6146,7 +6416,7 @@
         <v>850000</v>
       </c>
       <c r="G276" s="2">
-        <v>10665975</v>
+        <v>1915975</v>
       </c>
     </row>
     <row r="277" spans="1:7">
@@ -6166,7 +6436,7 @@
         <v>18500</v>
       </c>
       <c r="G277" s="2">
-        <v>10647475</v>
+        <v>1897475</v>
       </c>
     </row>
     <row r="278" spans="1:7">
@@ -6186,7 +6456,7 @@
         <v>144000</v>
       </c>
       <c r="G278" s="2">
-        <v>10503475</v>
+        <v>1753475</v>
       </c>
     </row>
     <row r="279" spans="1:7">
@@ -6206,7 +6476,7 @@
         <v>120000</v>
       </c>
       <c r="G279" s="2">
-        <v>10623475</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="280" spans="1:7">
@@ -6226,7 +6496,7 @@
         <v>10000</v>
       </c>
       <c r="G280" s="2">
-        <v>10613475</v>
+        <v>1850000</v>
       </c>
     </row>
     <row r="281" spans="1:7">
@@ -6243,10 +6513,10 @@
         <v>7</v>
       </c>
       <c r="E281" s="2">
-        <v>6000000</v>
+        <v>1250000</v>
       </c>
       <c r="G281" s="2">
-        <v>4613475</v>
+        <v>1806000</v>
       </c>
     </row>
     <row r="282" spans="1:7">
@@ -6266,7 +6536,7 @@
         <v>600000</v>
       </c>
       <c r="G282" s="2">
-        <v>4013475</v>
+        <v>1706000</v>
       </c>
     </row>
     <row r="283" spans="1:7">
@@ -6283,10 +6553,10 @@
         <v>7</v>
       </c>
       <c r="F283" s="2">
-        <v>4500000</v>
+        <v>120000</v>
       </c>
       <c r="G283" s="2">
-        <v>8513475</v>
+        <v>1871000</v>
       </c>
     </row>
     <row r="284" spans="1:7">
@@ -6306,7 +6576,7 @@
         <v>12000</v>
       </c>
       <c r="G284" s="2">
-        <v>8525475</v>
+        <v>1831000</v>
       </c>
     </row>
     <row r="285" spans="1:7">
@@ -6326,7 +6596,7 @@
         <v>48000</v>
       </c>
       <c r="G285" s="2">
-        <v>8477475</v>
+        <v>1769000</v>
       </c>
     </row>
     <row r="286" spans="1:7">
@@ -6346,7 +6616,7 @@
         <v>1000000</v>
       </c>
       <c r="G286" s="2">
-        <v>3000000</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="287" spans="1:7">
@@ -6366,7 +6636,7 @@
         <v>850000</v>
       </c>
       <c r="G287" s="2">
-        <v>3850000</v>
+        <v>2334000</v>
       </c>
     </row>
     <row r="288" spans="1:7">
@@ -6386,7 +6656,7 @@
         <v>44000</v>
       </c>
       <c r="G288" s="2">
-        <v>3806000</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="289" spans="1:7">
@@ -6406,7 +6676,7 @@
         <v>100000</v>
       </c>
       <c r="G289" s="2">
-        <v>3706000</v>
+        <v>1206000</v>
       </c>
     </row>
     <row r="290" spans="1:7">
@@ -6426,7 +6696,7 @@
         <v>165000</v>
       </c>
       <c r="G290" s="2">
-        <v>3871000</v>
+        <v>1371000</v>
       </c>
     </row>
     <row r="291" spans="1:7">
@@ -6446,7 +6716,7 @@
         <v>40000</v>
       </c>
       <c r="G291" s="2">
-        <v>3831000</v>
+        <v>1331000</v>
       </c>
     </row>
     <row r="292" spans="1:7">
@@ -6466,7 +6736,7 @@
         <v>62000</v>
       </c>
       <c r="G292" s="2">
-        <v>3769000</v>
+        <v>1269000</v>
       </c>
     </row>
     <row r="293" spans="1:7">
@@ -6486,7 +6756,7 @@
         <v>815000</v>
       </c>
       <c r="G293" s="2">
-        <v>4584000</v>
+        <v>2084000</v>
       </c>
     </row>
     <row r="294" spans="1:7">
@@ -6506,7 +6776,7 @@
         <v>250000</v>
       </c>
       <c r="G294" s="2">
-        <v>4334000</v>
+        <v>1834000</v>
       </c>
     </row>
     <row r="295" spans="1:7">
@@ -6526,7 +6796,7 @@
         <v>3000000</v>
       </c>
       <c r="G295" s="2">
-        <v>7334000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="296" spans="1:7">
@@ -6546,7 +6816,7 @@
         <v>180025</v>
       </c>
       <c r="G296" s="2">
-        <v>7153975</v>
+        <v>1850000</v>
       </c>
     </row>
     <row r="297" spans="1:7">
@@ -6566,7 +6836,7 @@
         <v>64000</v>
       </c>
       <c r="G297" s="2">
-        <v>7089975</v>
+        <v>1806000</v>
       </c>
     </row>
     <row r="298" spans="1:7">
@@ -6586,7 +6856,7 @@
         <v>29000</v>
       </c>
       <c r="G298" s="2">
-        <v>7060975</v>
+        <v>1706000</v>
       </c>
     </row>
     <row r="299" spans="1:7">
@@ -6606,7 +6876,7 @@
         <v>125000</v>
       </c>
       <c r="G299" s="2">
-        <v>7185975</v>
+        <v>1871000</v>
       </c>
     </row>
     <row r="300" spans="1:7">
@@ -6626,7 +6896,7 @@
         <v>1800000</v>
       </c>
       <c r="G300" s="2">
-        <v>5385975</v>
+        <v>1831000</v>
       </c>
     </row>
     <row r="301" spans="1:7">
@@ -6646,7 +6916,7 @@
         <v>25000</v>
       </c>
       <c r="G301" s="2">
-        <v>5360975</v>
+        <v>1769000</v>
       </c>
     </row>
     <row r="302" spans="1:7">
@@ -6663,10 +6933,10 @@
         <v>7</v>
       </c>
       <c r="F302" s="2">
-        <v>2200000</v>
+        <v>220000</v>
       </c>
       <c r="G302" s="2">
-        <v>7560975</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="303" spans="1:7">
@@ -6686,7 +6956,7 @@
         <v>120000</v>
       </c>
       <c r="G303" s="2">
-        <v>7440975</v>
+        <v>2334000</v>
       </c>
     </row>
     <row r="304" spans="1:7">
@@ -6706,7 +6976,7 @@
         <v>75000</v>
       </c>
       <c r="G304" s="2">
-        <v>7515975</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="305" spans="1:7">
@@ -6726,7 +6996,7 @@
         <v>850000</v>
       </c>
       <c r="G305" s="2">
-        <v>6665975</v>
+        <v>2185975</v>
       </c>
     </row>
     <row r="306" spans="1:7">
@@ -6746,7 +7016,7 @@
         <v>18500</v>
       </c>
       <c r="G306" s="2">
-        <v>6647475</v>
+        <v>2167475</v>
       </c>
     </row>
     <row r="307" spans="1:7">
@@ -6766,7 +7036,7 @@
         <v>144000</v>
       </c>
       <c r="G307" s="2">
-        <v>6503475</v>
+        <v>2023475</v>
       </c>
     </row>
     <row r="308" spans="1:7">
@@ -6786,7 +7056,7 @@
         <v>120000</v>
       </c>
       <c r="G308" s="2">
-        <v>6623475</v>
+        <v>2143475</v>
       </c>
     </row>
     <row r="309" spans="1:7">
@@ -6806,7 +7076,7 @@
         <v>10000</v>
       </c>
       <c r="G309" s="2">
-        <v>6613475</v>
+        <v>2133475</v>
       </c>
     </row>
     <row r="310" spans="1:7">
@@ -6823,10 +7093,10 @@
         <v>7</v>
       </c>
       <c r="E310" s="2">
-        <v>6000000</v>
+        <v>116000</v>
       </c>
       <c r="G310" s="2">
-        <v>613475</v>
+        <v>2017475</v>
       </c>
     </row>
     <row r="311" spans="1:7">
@@ -6846,7 +7116,7 @@
         <v>600000</v>
       </c>
       <c r="G311" s="2">
-        <v>13475</v>
+        <v>1417475</v>
       </c>
     </row>
     <row r="312" spans="1:7">
@@ -6863,10 +7133,10 @@
         <v>7</v>
       </c>
       <c r="F312" s="2">
-        <v>4500000</v>
+        <v>450000</v>
       </c>
       <c r="G312" s="2">
-        <v>4513475</v>
+        <v>1867475</v>
       </c>
     </row>
     <row r="313" spans="1:7">
@@ -6886,7 +7156,7 @@
         <v>12000</v>
       </c>
       <c r="G313" s="2">
-        <v>4525475</v>
+        <v>1879475</v>
       </c>
     </row>
     <row r="314" spans="1:7">
@@ -6906,8 +7176,8 @@
         <v>48000</v>
       </c>
       <c r="F314" s="5"/>
-      <c r="G314" s="5">
-        <v>4477475</v>
+      <c r="G314" s="2">
+        <v>2000000</v>
       </c>
     </row>
     <row r="315" spans="1:7">
@@ -6927,7 +7197,7 @@
         <v>1000000</v>
       </c>
       <c r="G315" s="2">
-        <v>11000000</v>
+        <v>1850000</v>
       </c>
     </row>
     <row r="316" spans="1:7">
@@ -6947,7 +7217,7 @@
         <v>850000</v>
       </c>
       <c r="G316" s="2">
-        <v>11850000</v>
+        <v>1806000</v>
       </c>
     </row>
     <row r="317" spans="1:7">
@@ -6967,7 +7237,7 @@
         <v>450000</v>
       </c>
       <c r="G317" s="2">
-        <v>11400000</v>
+        <v>1706000</v>
       </c>
     </row>
     <row r="318" spans="1:7">
@@ -6987,7 +7257,7 @@
         <v>100000</v>
       </c>
       <c r="G318" s="2">
-        <v>11300000</v>
+        <v>1871000</v>
       </c>
     </row>
     <row r="319" spans="1:7">
@@ -7007,7 +7277,7 @@
         <v>165000</v>
       </c>
       <c r="G319" s="2">
-        <v>11465000</v>
+        <v>1831000</v>
       </c>
     </row>
     <row r="320" spans="1:7">
@@ -7027,7 +7297,7 @@
         <v>40000</v>
       </c>
       <c r="G320" s="2">
-        <v>11425000</v>
+        <v>1769000</v>
       </c>
     </row>
     <row r="321" spans="1:7">
@@ -7047,7 +7317,7 @@
         <v>620000</v>
       </c>
       <c r="G321" s="2">
-        <v>10805000</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="322" spans="1:7">
@@ -7067,7 +7337,7 @@
         <v>815000</v>
       </c>
       <c r="G322" s="2">
-        <v>11620000</v>
+        <v>2334000</v>
       </c>
     </row>
     <row r="323" spans="1:7">
@@ -7087,7 +7357,7 @@
         <v>250000</v>
       </c>
       <c r="G323" s="2">
-        <v>11370000</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="324" spans="1:7">
@@ -7107,7 +7377,7 @@
         <v>3000000</v>
       </c>
       <c r="G324" s="2">
-        <v>14370000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="325" spans="1:7">
@@ -7127,7 +7397,7 @@
         <v>180025</v>
       </c>
       <c r="G325" s="2">
-        <v>14189975</v>
+        <v>1850000</v>
       </c>
     </row>
     <row r="326" spans="1:7">
@@ -7147,7 +7417,7 @@
         <v>64000</v>
       </c>
       <c r="G326" s="2">
-        <v>14125975</v>
+        <v>1806000</v>
       </c>
     </row>
     <row r="327" spans="1:7">
@@ -7167,7 +7437,7 @@
         <v>29000</v>
       </c>
       <c r="G327" s="2">
-        <v>14096975</v>
+        <v>1706000</v>
       </c>
     </row>
     <row r="328" spans="1:7">
@@ -7187,7 +7457,7 @@
         <v>125000</v>
       </c>
       <c r="G328" s="2">
-        <v>14221975</v>
+        <v>1871000</v>
       </c>
     </row>
     <row r="329" spans="1:7">
@@ -7207,7 +7477,7 @@
         <v>1800000</v>
       </c>
       <c r="G329" s="2">
-        <v>12421975</v>
+        <v>1831000</v>
       </c>
     </row>
     <row r="330" spans="1:7">
@@ -7224,10 +7494,10 @@
         <v>7</v>
       </c>
       <c r="E330" s="2">
-        <v>2500000</v>
+        <v>25000</v>
       </c>
       <c r="G330" s="2">
-        <v>9921975</v>
+        <v>1769000</v>
       </c>
     </row>
     <row r="331" spans="1:7">
@@ -7247,7 +7517,7 @@
         <v>2200000</v>
       </c>
       <c r="G331" s="2">
-        <v>12121975</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="332" spans="1:7">
@@ -7267,7 +7537,7 @@
         <v>120000</v>
       </c>
       <c r="G332" s="2">
-        <v>12001975</v>
+        <v>1850000</v>
       </c>
     </row>
     <row r="333" spans="1:7">
@@ -7287,7 +7557,7 @@
         <v>75000</v>
       </c>
       <c r="G333" s="2">
-        <v>12076975</v>
+        <v>1806000</v>
       </c>
     </row>
     <row r="334" spans="1:7">
@@ -7307,7 +7577,7 @@
         <v>850000</v>
       </c>
       <c r="G334" s="2">
-        <v>11226975</v>
+        <v>1706000</v>
       </c>
     </row>
     <row r="335" spans="1:7">
@@ -7327,7 +7597,7 @@
         <v>18500</v>
       </c>
       <c r="G335" s="2">
-        <v>11208475</v>
+        <v>1871000</v>
       </c>
     </row>
     <row r="336" spans="1:7">
@@ -7347,7 +7617,7 @@
         <v>144000</v>
       </c>
       <c r="G336" s="2">
-        <v>11064475</v>
+        <v>1831000</v>
       </c>
     </row>
     <row r="337" spans="1:7">
@@ -7367,7 +7637,7 @@
         <v>250000</v>
       </c>
       <c r="G337" s="2">
-        <v>11314475</v>
+        <v>1769000</v>
       </c>
     </row>
     <row r="338" spans="1:7">
@@ -7387,7 +7657,7 @@
         <v>10000</v>
       </c>
       <c r="G338" s="2">
-        <v>11304475</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="339" spans="1:7">
@@ -7404,10 +7674,10 @@
         <v>7</v>
       </c>
       <c r="E339" s="2">
-        <v>6000000</v>
+        <v>750000</v>
       </c>
       <c r="G339" s="2">
-        <v>5304475</v>
+        <v>2334000</v>
       </c>
     </row>
     <row r="340" spans="1:7">
@@ -7427,7 +7697,7 @@
         <v>600000</v>
       </c>
       <c r="G340" s="2">
-        <v>4704475</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="341" spans="1:7">
@@ -7444,10 +7714,10 @@
         <v>7</v>
       </c>
       <c r="F341" s="2">
-        <v>4500000</v>
+        <v>45000</v>
       </c>
       <c r="G341" s="2">
-        <v>9204475</v>
+        <v>1831000</v>
       </c>
     </row>
     <row r="342" spans="1:7">
@@ -7467,7 +7737,7 @@
         <v>120000</v>
       </c>
       <c r="G342" s="2">
-        <v>9324475</v>
+        <v>1769000</v>
       </c>
     </row>
     <row r="343" spans="1:7">
@@ -7487,8 +7757,8 @@
         <v>560000</v>
       </c>
       <c r="F343" s="5"/>
-      <c r="G343" s="5">
-        <v>8764475</v>
+      <c r="G343" s="2">
+        <v>2584000</v>
       </c>
     </row>
     <row r="344" spans="1:7">
@@ -7505,10 +7775,10 @@
         <v>7</v>
       </c>
       <c r="E344" s="2">
-        <v>2500000</v>
+        <v>25000</v>
       </c>
       <c r="G344" s="2">
-        <v>3500000</v>
+        <v>2334000</v>
       </c>
     </row>
     <row r="345" spans="1:7">
@@ -7528,7 +7798,7 @@
         <v>850000</v>
       </c>
       <c r="G345" s="2">
-        <v>4350000</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="346" spans="1:7">
@@ -7548,7 +7818,7 @@
         <v>450000</v>
       </c>
       <c r="G346" s="2">
-        <v>3900000</v>
+        <v>1625000</v>
       </c>
     </row>
     <row r="347" spans="1:7">
@@ -7568,7 +7838,7 @@
         <v>100000</v>
       </c>
       <c r="G347" s="2">
-        <v>3800000</v>
+        <v>1525000</v>
       </c>
     </row>
     <row r="348" spans="1:7">
@@ -7588,7 +7858,7 @@
         <v>165000</v>
       </c>
       <c r="G348" s="2">
-        <v>3965000</v>
+        <v>1690000</v>
       </c>
     </row>
     <row r="349" spans="1:7">
@@ -7608,7 +7878,7 @@
         <v>40000</v>
       </c>
       <c r="G349" s="2">
-        <v>3925000</v>
+        <v>1650000</v>
       </c>
     </row>
     <row r="350" spans="1:7">
@@ -7628,7 +7898,7 @@
         <v>620000</v>
       </c>
       <c r="G350" s="2">
-        <v>3305000</v>
+        <v>1831000</v>
       </c>
     </row>
     <row r="351" spans="1:7">
@@ -7648,7 +7918,7 @@
         <v>815000</v>
       </c>
       <c r="G351" s="2">
-        <v>4120000</v>
+        <v>1845000</v>
       </c>
     </row>
     <row r="352" spans="1:7">
@@ -7668,7 +7938,7 @@
         <v>250000</v>
       </c>
       <c r="G352" s="2">
-        <v>3870000</v>
+        <v>1595000</v>
       </c>
     </row>
     <row r="353" spans="1:7">
@@ -7685,10 +7955,10 @@
         <v>7</v>
       </c>
       <c r="F353" s="2">
-        <v>3000000</v>
+        <v>300000</v>
       </c>
       <c r="G353" s="2">
-        <v>6870000</v>
+        <v>1895000</v>
       </c>
     </row>
     <row r="354" spans="1:7">
@@ -7708,7 +7978,7 @@
         <v>180025</v>
       </c>
       <c r="G354" s="2">
-        <v>6689975</v>
+        <v>1714975</v>
       </c>
     </row>
     <row r="355" spans="1:7">
@@ -7728,7 +7998,7 @@
         <v>64000</v>
       </c>
       <c r="G355" s="2">
-        <v>6625975</v>
+        <v>1650975</v>
       </c>
     </row>
     <row r="356" spans="1:7">
@@ -7748,7 +8018,7 @@
         <v>29000</v>
       </c>
       <c r="G356" s="2">
-        <v>6596975</v>
+        <v>1621975</v>
       </c>
     </row>
     <row r="357" spans="1:7">
@@ -7768,7 +8038,7 @@
         <v>125000</v>
       </c>
       <c r="G357" s="2">
-        <v>6721975</v>
+        <v>1746975</v>
       </c>
     </row>
     <row r="358" spans="1:7">
@@ -7785,10 +8055,10 @@
         <v>7</v>
       </c>
       <c r="E358" s="2">
-        <v>1800000</v>
+        <v>180000</v>
       </c>
       <c r="G358" s="2">
-        <v>4921975</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="359" spans="1:7">
@@ -7805,10 +8075,10 @@
         <v>7</v>
       </c>
       <c r="E359" s="2">
-        <v>2500000</v>
+        <v>250000</v>
       </c>
       <c r="G359" s="2">
-        <v>2421975</v>
+        <v>1831000</v>
       </c>
     </row>
     <row r="360" spans="1:7">
@@ -7828,7 +8098,7 @@
         <v>2200000</v>
       </c>
       <c r="G360" s="2">
-        <v>4621975</v>
+        <v>1769000</v>
       </c>
     </row>
     <row r="361" spans="1:7">
@@ -7848,7 +8118,7 @@
         <v>120000</v>
       </c>
       <c r="G361" s="2">
-        <v>4501975</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="362" spans="1:7">
@@ -7868,7 +8138,7 @@
         <v>75000</v>
       </c>
       <c r="G362" s="2">
-        <v>4576975</v>
+        <v>2334000</v>
       </c>
     </row>
     <row r="363" spans="1:7">
@@ -7888,7 +8158,7 @@
         <v>850000</v>
       </c>
       <c r="G363" s="2">
-        <v>3726975</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="364" spans="1:7">
@@ -7908,7 +8178,7 @@
         <v>18500</v>
       </c>
       <c r="G364" s="2">
-        <v>3708475</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="365" spans="1:7">
@@ -7928,7 +8198,7 @@
         <v>144000</v>
       </c>
       <c r="G365" s="2">
-        <v>3564475</v>
+        <v>1831000</v>
       </c>
     </row>
     <row r="366" spans="1:7">
@@ -7945,10 +8215,10 @@
         <v>7</v>
       </c>
       <c r="F366" s="2">
-        <v>2500000</v>
+        <v>350000</v>
       </c>
       <c r="G366" s="2">
-        <v>6064475</v>
+        <v>1769000</v>
       </c>
     </row>
     <row r="367" spans="1:7">
@@ -7968,7 +8238,7 @@
         <v>10000</v>
       </c>
       <c r="G367" s="2">
-        <v>6054475</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="368" spans="1:7">
@@ -7985,10 +8255,10 @@
         <v>7</v>
       </c>
       <c r="E368" s="2">
-        <v>6000000</v>
+        <v>290000</v>
       </c>
       <c r="G368" s="2">
-        <v>54475</v>
+        <v>2334000</v>
       </c>
     </row>
     <row r="369" spans="1:7">
@@ -8008,7 +8278,7 @@
         <v>125000</v>
       </c>
       <c r="G369" s="2">
-        <v>179475</v>
+        <v>2584000</v>
       </c>
     </row>
     <row r="370" spans="1:7">
@@ -8025,10 +8295,10 @@
         <v>7</v>
       </c>
       <c r="F370" s="2">
-        <v>4500000</v>
+        <v>330000</v>
       </c>
       <c r="G370" s="2">
-        <v>4679475</v>
+        <v>1625000</v>
       </c>
     </row>
     <row r="371" spans="1:7">
@@ -8048,7 +8318,7 @@
         <v>120000</v>
       </c>
       <c r="G371" s="2">
-        <v>4799475</v>
+        <v>1525000</v>
       </c>
     </row>
     <row r="372" spans="1:7">
@@ -8069,7 +8339,7 @@
       </c>
       <c r="F372" s="5"/>
       <c r="G372" s="5">
-        <v>4239475</v>
+        <v>2524475</v>
       </c>
     </row>
   </sheetData>
@@ -8082,25 +8352,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -8125,10 +8398,25 @@
       <c r="H1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="6">
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
         <v>12400528</v>
+      </c>
+      <c r="B2">
+        <v>111222333</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -8136,10 +8424,37 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="6">
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
         <v>12605077</v>
+      </c>
+      <c r="B3">
+        <v>111222334</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -8147,10 +8462,37 @@
       <c r="D3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="6">
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
         <v>12605088</v>
+      </c>
+      <c r="B4">
+        <v>111222335</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -8158,10 +8500,37 @@
       <c r="D4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="6">
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
         <v>12605122</v>
+      </c>
+      <c r="B5">
+        <v>111222336</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -8169,10 +8538,37 @@
       <c r="D5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="6">
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
         <v>12605144</v>
+      </c>
+      <c r="B6">
+        <v>111222337</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -8180,10 +8576,37 @@
       <c r="D6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="6">
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6">
+        <v>32</v>
+      </c>
+      <c r="J6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
         <v>12605155</v>
+      </c>
+      <c r="B7">
+        <v>111222338</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
@@ -8191,10 +8614,37 @@
       <c r="D7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="6">
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K7" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
         <v>12605199</v>
+      </c>
+      <c r="B8">
+        <v>111222339</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
@@ -8202,10 +8652,37 @@
       <c r="D8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="6">
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
         <v>12605201</v>
+      </c>
+      <c r="B9">
+        <v>111222340</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
@@ -8213,10 +8690,37 @@
       <c r="D9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="6">
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9">
+        <v>35</v>
+      </c>
+      <c r="J9" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
         <v>12605222</v>
+      </c>
+      <c r="B10">
+        <v>111222341</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
@@ -8224,10 +8728,37 @@
       <c r="D10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="6">
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10">
+        <v>45</v>
+      </c>
+      <c r="J10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K10" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
         <v>12605233</v>
+      </c>
+      <c r="B11">
+        <v>111222342</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
@@ -8235,10 +8766,37 @@
       <c r="D11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="6">
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11">
+        <v>62</v>
+      </c>
+      <c r="J11" t="s">
+        <v>89</v>
+      </c>
+      <c r="K11" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
         <v>12605244</v>
+      </c>
+      <c r="B12">
+        <v>111222343</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -8246,10 +8804,37 @@
       <c r="D12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="6">
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12">
+        <v>51</v>
+      </c>
+      <c r="J12" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
         <v>12605266</v>
+      </c>
+      <c r="B13">
+        <v>111222344</v>
       </c>
       <c r="C13" t="s">
         <v>36</v>
@@ -8257,8 +8842,268 @@
       <c r="D13" t="s">
         <v>37</v>
       </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" t="s">
+        <v>80</v>
+      </c>
+      <c r="I13">
+        <v>48</v>
+      </c>
+      <c r="J13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" t="s">
+        <v>85</v>
+      </c>
+      <c r="L13" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>12400528</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>12605077</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>12605088</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>12605122</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1000</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>12605144</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="6">
+        <v>25000</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>12605155</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="6">
+        <v>25000</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>12605199</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="6">
+        <v>25000</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>12605201</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="6">
+        <v>25000</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>12605222</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="6">
+        <v>500000</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>12605233</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="6">
+        <v>500000</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>12605244</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="6">
+        <v>500000</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>12605266</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="6">
+        <v>500000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cluster | Kyc Clustering -v6
</commit_message>
<xml_diff>
--- a/Data/inputs.xlsx
+++ b/Data/inputs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="95">
   <si>
     <t>TRAN_DT</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t>DENTIST</t>
+  </si>
+  <si>
+    <t>INCOME</t>
   </si>
 </sst>
 </file>
@@ -362,6 +365,9 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -399,9 +405,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     </dxf>
     <dxf>
       <font>
@@ -556,15 +559,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:L13" totalsRowShown="0">
-  <autoFilter ref="A1:L13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:M13" totalsRowShown="0">
+  <autoFilter ref="A1:M13">
     <filterColumn colId="8"/>
     <filterColumn colId="9"/>
     <filterColumn colId="10"/>
     <filterColumn colId="11"/>
+    <filterColumn colId="12"/>
   </autoFilter>
-  <tableColumns count="12">
-    <tableColumn id="1" name="ACC_ID" dataDxfId="0"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="ACC_ID" dataDxfId="2"/>
     <tableColumn id="2" name="SSN"/>
     <tableColumn id="3" name="FIRST_NAME"/>
     <tableColumn id="4" name="LAST_NAME"/>
@@ -576,6 +580,7 @@
     <tableColumn id="10" name="MARITAL"/>
     <tableColumn id="11" name="GENDER"/>
     <tableColumn id="12" name="OCCUPATION"/>
+    <tableColumn id="13" name="INCOME"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -585,10 +590,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D13" totalsRowShown="0">
   <autoFilter ref="A1:D13"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="ACC_ID" dataDxfId="2"/>
+    <tableColumn id="1" name="ACC_ID" dataDxfId="1"/>
     <tableColumn id="2" name="CLUSTER"/>
     <tableColumn id="3" name="AVE_BAL"/>
-    <tableColumn id="4" name="AVE_TXN" dataDxfId="1"/>
+    <tableColumn id="4" name="AVE_TXN" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -882,7 +887,7 @@
   <dimension ref="A1:G372"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C256" sqref="C256"/>
+      <selection activeCell="A257" sqref="A257:G258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8352,10 +8357,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L13"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8373,7 +8378,7 @@
     <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -8410,8 +8415,11 @@
       <c r="L1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>12400528</v>
       </c>
@@ -8448,8 +8456,11 @@
       <c r="L2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>12605077</v>
       </c>
@@ -8486,8 +8497,11 @@
       <c r="L3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3">
+        <v>85000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>12605088</v>
       </c>
@@ -8524,8 +8538,11 @@
       <c r="L4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <v>112000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>12605122</v>
       </c>
@@ -8562,8 +8579,11 @@
       <c r="L5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <v>98000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>12605144</v>
       </c>
@@ -8600,8 +8620,11 @@
       <c r="L6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <v>690000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>12605155</v>
       </c>
@@ -8638,8 +8661,11 @@
       <c r="L7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>12605199</v>
       </c>
@@ -8676,8 +8702,11 @@
       <c r="L8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8">
+        <v>780000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>12605201</v>
       </c>
@@ -8714,8 +8743,11 @@
       <c r="L9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9">
+        <v>720000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>12605222</v>
       </c>
@@ -8752,8 +8784,11 @@
       <c r="L10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>12605233</v>
       </c>
@@ -8790,8 +8825,11 @@
       <c r="L11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11">
+        <v>1150000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>12605244</v>
       </c>
@@ -8828,8 +8866,11 @@
       <c r="L12" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12">
+        <v>1005000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>12605266</v>
       </c>
@@ -8865,6 +8906,9 @@
       </c>
       <c r="L13" t="s">
         <v>91</v>
+      </c>
+      <c r="M13">
+        <v>1075000</v>
       </c>
     </row>
   </sheetData>
@@ -8880,7 +8924,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>